<commit_message>
made so that the excel file saved the seconds spent studying in numbers instead of text
</commit_message>
<xml_diff>
--- a/PYTHON/test.xlsx
+++ b/PYTHON/test.xlsx
@@ -1,41 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\GitHub\StudyTImeInExcel\PYTHON\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923EBA7A-16A9-4DB1-AB24-0FD52DBDA7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time(s)</t>
+  </si>
+  <si>
+    <t>25/01/2024</t>
+  </si>
+  <si>
+    <t>26/01/2024</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -53,82 +75,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,51 +381,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="12.42578125" customWidth="1" min="2" max="2"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Time(s)</t>
-        </is>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>21.0</t>
-        </is>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>21</v>
       </c>
     </row>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6">
-      <c r="E6" s="1" t="n"/>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
cleaned the code, a 3rd column with hours and some code to add a chart
</commit_message>
<xml_diff>
--- a/PYTHON/test.xlsx
+++ b/PYTHON/test.xlsx
@@ -1,63 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\GitHub\StudyTImeInExcel\PYTHON\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923EBA7A-16A9-4DB1-AB24-0FD52DBDA7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time(s)</t>
-  </si>
-  <si>
-    <t>25/01/2024</t>
-  </si>
-  <si>
-    <t>26/01/2024</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,26 +45,357 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Time spent studying</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!D2</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$3</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$D$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Time (h)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Time spent studying</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!D2</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$3</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$D$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Time (h)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,46 +682,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E6"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col width="12.42578125" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
+    <row r="1"/>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Time(s)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Time(h)</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>26/01/2024</t>
+        </is>
       </c>
-      <c r="C3" s="3">
-        <v>21</v>
+      <c r="C3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.004166666666666667</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
+    <row r="4">
+      <c r="C4" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>